<commit_message>
final tables had space. Now "_" since not supported by bookdown
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\GenerateDAG\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4686A1-2DAD-4410-9091-50984BC4727A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D230B1-25EB-4F69-AC55-8D07C01EC61F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,30 +191,12 @@
     <t>06_T4_20_create_D5_IR_background_std</t>
   </si>
   <si>
-    <t>Table 1</t>
-  </si>
-  <si>
     <t>07_T5_10_final_tables</t>
   </si>
   <si>
     <t>g_export/Dummy tables</t>
   </si>
   <si>
-    <t>Table 2</t>
-  </si>
-  <si>
-    <t>Table 3</t>
-  </si>
-  <si>
-    <t>Table 4</t>
-  </si>
-  <si>
-    <t>Table 5</t>
-  </si>
-  <si>
-    <t>Table 6</t>
-  </si>
-  <si>
     <t>parameter in the table name</t>
   </si>
   <si>
@@ -513,6 +495,24 @@
   </si>
   <si>
     <t>slug</t>
+  </si>
+  <si>
+    <t>Table_1</t>
+  </si>
+  <si>
+    <t>Table_2</t>
+  </si>
+  <si>
+    <t>Table_3</t>
+  </si>
+  <si>
+    <t>Table_4</t>
+  </si>
+  <si>
+    <t>Table_5</t>
+  </si>
+  <si>
+    <t>Table_6</t>
   </si>
 </sst>
 </file>
@@ -939,7 +939,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +978,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1175,16 +1175,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1245,86 +1245,86 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
         <v>57</v>
       </c>
-      <c r="D20" t="s">
-        <v>58</v>
-      </c>
       <c r="E20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="C21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
         <v>57</v>
       </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
       <c r="E21" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>61</v>
+        <v>161</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
         <v>57</v>
       </c>
-      <c r="D22" t="s">
-        <v>58</v>
-      </c>
       <c r="E22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>62</v>
+        <v>162</v>
       </c>
       <c r="C23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
         <v>57</v>
       </c>
-      <c r="D23" t="s">
-        <v>58</v>
-      </c>
       <c r="E23" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>63</v>
+        <v>163</v>
       </c>
       <c r="C24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
         <v>57</v>
       </c>
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
       <c r="E24" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1350,16 +1350,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1367,10 +1367,10 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1378,10 +1378,10 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1389,7 +1389,7 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1397,7 +1397,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1405,144 +1405,144 @@
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1558,7 +1558,7 @@
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1566,7 +1566,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1574,7 +1574,7 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
         <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1598,634 +1598,634 @@
         <v>46</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
         <v>97</v>
       </c>
-      <c r="B28" t="s">
-        <v>103</v>
-      </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C51" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C57" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C58" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C59" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C60" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C61" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C62" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C63" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C64" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C65" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C68" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B69" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C69" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C70" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C71" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C72" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C73" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C74" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B75" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C75" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C76" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C77" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B78" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C78" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C79" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B80" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C80" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2243,18 +2243,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6dac44d48b4406d5c320fe911a853389">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="183e839aabd2ef2c305af4a754f6d8de" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2499,6 +2487,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
@@ -2508,17 +2508,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8527D96-6D0B-44E8-B45B-3BF8C6261239}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2535,4 +2524,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
table 1, etc without spaces with "_"
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20403"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\GenerateDAG\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\GenerateDAG\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE185CEA-C4F6-4EDB-A612-66C54E1B6E34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -190,30 +191,12 @@
     <t>06_T4_20_create_D5_IR_background_std</t>
   </si>
   <si>
-    <t>Table 1</t>
-  </si>
-  <si>
     <t>07_T5_10_final_tables</t>
   </si>
   <si>
     <t>g_export/Dummy tables</t>
   </si>
   <si>
-    <t>Table 2</t>
-  </si>
-  <si>
-    <t>Table 3</t>
-  </si>
-  <si>
-    <t>Table 4</t>
-  </si>
-  <si>
-    <t>Table 5</t>
-  </si>
-  <si>
-    <t>Table 6</t>
-  </si>
-  <si>
     <t>parameter in the table name</t>
   </si>
   <si>
@@ -512,12 +495,30 @@
   </si>
   <si>
     <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_study_population_with_covariates D5_IR_background D5_IR_background_std</t>
+  </si>
+  <si>
+    <t>Table_1</t>
+  </si>
+  <si>
+    <t>Table_2</t>
+  </si>
+  <si>
+    <t>Table_3</t>
+  </si>
+  <si>
+    <t>Table_4</t>
+  </si>
+  <si>
+    <t>Table_5</t>
+  </si>
+  <si>
+    <t>Table_6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,7 +621,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -931,27 +932,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19:E24"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.5546875" customWidth="1"/>
-    <col min="3" max="3" width="53.109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="49.33203125" customWidth="1"/>
-    <col min="5" max="5" width="131.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" customWidth="1"/>
+    <col min="5" max="5" width="131.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,10 +978,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -997,7 +998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1048,7 +1049,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1065,7 +1066,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
@@ -1096,7 +1097,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>39</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>41</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>43</v>
       </c>
@@ -1172,21 +1173,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>48</v>
       </c>
@@ -1197,10 +1198,10 @@
         <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>50</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>52</v>
       </c>
@@ -1228,7 +1229,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>54</v>
       </c>
@@ -1242,88 +1243,88 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
       <c r="E19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="13" t="s">
+      <c r="C24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
         <v>57</v>
       </c>
-      <c r="D20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
       <c r="E24" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1333,898 +1334,898 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
         <v>97</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="s">
         <v>98</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
         <v>100</v>
       </c>
-      <c r="C25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
         <v>101</v>
       </c>
-      <c r="C26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
         <v>102</v>
       </c>
-      <c r="C27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
         <v>103</v>
       </c>
-      <c r="C28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s">
         <v>104</v>
       </c>
-      <c r="C29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
         <v>105</v>
       </c>
-      <c r="C30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
         <v>106</v>
       </c>
-      <c r="C31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
         <v>107</v>
       </c>
-      <c r="C32" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
         <v>108</v>
       </c>
-      <c r="C33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
         <v>109</v>
       </c>
-      <c r="C34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" t="s">
         <v>110</v>
       </c>
-      <c r="C35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
         <v>111</v>
       </c>
-      <c r="C36" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
         <v>112</v>
       </c>
-      <c r="C37" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
         <v>113</v>
       </c>
-      <c r="C38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
         <v>114</v>
       </c>
-      <c r="C39" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
         <v>115</v>
       </c>
-      <c r="C40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
         <v>116</v>
       </c>
-      <c r="C41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" t="s">
         <v>117</v>
       </c>
-      <c r="C42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C48" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
         <v>118</v>
       </c>
-      <c r="C43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" t="s">
         <v>119</v>
       </c>
-      <c r="C44" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" t="s">
         <v>120</v>
       </c>
-      <c r="C45" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" t="s">
         <v>121</v>
       </c>
-      <c r="C46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" t="s">
         <v>122</v>
       </c>
-      <c r="C47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" t="s">
         <v>123</v>
       </c>
-      <c r="C48" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" t="s">
         <v>124</v>
       </c>
-      <c r="C49" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" t="s">
         <v>125</v>
       </c>
-      <c r="C50" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" t="s">
         <v>126</v>
       </c>
-      <c r="C51" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" t="s">
         <v>127</v>
       </c>
-      <c r="C52" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="C58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" t="s">
         <v>128</v>
       </c>
-      <c r="C53" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" t="s">
         <v>129</v>
       </c>
-      <c r="C54" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" t="s">
         <v>130</v>
       </c>
-      <c r="C55" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" t="s">
         <v>131</v>
       </c>
-      <c r="C56" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" t="s">
         <v>132</v>
       </c>
-      <c r="C57" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C63" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" t="s">
         <v>133</v>
       </c>
-      <c r="C58" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" t="s">
         <v>134</v>
       </c>
-      <c r="C59" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" t="s">
         <v>135</v>
       </c>
-      <c r="C60" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67" t="s">
         <v>136</v>
       </c>
-      <c r="C61" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="C67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" t="s">
         <v>137</v>
       </c>
-      <c r="C62" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C68" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" t="s">
         <v>138</v>
       </c>
-      <c r="C63" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C69" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" t="s">
         <v>139</v>
       </c>
-      <c r="C64" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C70" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" t="s">
         <v>140</v>
       </c>
-      <c r="C65" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="C71" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" t="s">
         <v>141</v>
       </c>
-      <c r="C66" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="C72" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73" t="s">
         <v>142</v>
       </c>
-      <c r="C67" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="C73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" t="s">
         <v>143</v>
       </c>
-      <c r="C68" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="C74" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" t="s">
         <v>144</v>
       </c>
-      <c r="C69" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="C75" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76" t="s">
         <v>145</v>
       </c>
-      <c r="C70" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="C76" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" t="s">
         <v>146</v>
       </c>
-      <c r="C71" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="C77" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" t="s">
         <v>147</v>
       </c>
-      <c r="C72" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="C78" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79" t="s">
         <v>148</v>
       </c>
-      <c r="C73" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C79" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C74" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" t="s">
+      <c r="B80" t="s">
         <v>150</v>
       </c>
-      <c r="C75" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="C80" t="s">
         <v>151</v>
-      </c>
-      <c r="C76" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B77" t="s">
-        <v>152</v>
-      </c>
-      <c r="C77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B78" t="s">
-        <v>153</v>
-      </c>
-      <c r="C78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B79" t="s">
-        <v>154</v>
-      </c>
-      <c r="C79" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B80" t="s">
-        <v>156</v>
-      </c>
-      <c r="C80" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2242,6 +2243,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6dac44d48b4406d5c320fe911a853389">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="183e839aabd2ef2c305af4a754f6d8de" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2486,18 +2499,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
@@ -2507,6 +2508,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8527D96-6D0B-44E8-B45B-3BF8C6261239}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2523,15 +2535,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>